<commit_message>
fix: final result path
</commit_message>
<xml_diff>
--- a/data/final_results.xlsx
+++ b/data/final_results.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>does not provide a comparison or outcome related to extra-hepatic cancers</t>
+          <t>does not compare NAFLD patients with a control group</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>effects of moderate alcohol consumption on NAFLD</t>
+          <t>effects of moderate alcohol consumption</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -619,32 +619,32 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>The abstract discusses the effects of moderate alcohol consumption on NAFLD patients but does not address the incidence of extra-hepatic cancers or compare NAFLD patients to a non-NAFLD population. The focus is on liver fibrosis progression rather than cancer outcomes.</t>
+          <t>The abstract discusses moderate alcohol consumption's effects on NAFLD but does not address the incidence of extra-hepatic cancers or compare NAFLD patients with a non-NAFLD population. The focus is on liver fibrosis progression rather than cancer outcomes.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Patients with NAFLD are mentioned, but the abstract focuses on alcohol consumption's impact rather than cancer risks in NAFLD specifically.</t>
+          <t>Patients with NAFLD are mentioned, but the abstract focuses on alcohol consumption effects rather than cancer risks in NAFLD specifically.</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>The intervention involves observation of moderate alcohol consumption's effects, which is unrelated to managing NAFLD for cancer prevention.</t>
+          <t>The intervention pertains to moderate alcohol consumption and its impact on liver fibrosis, not observation or management of NAFLD related to cancer risks.</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>No comparison group involving non-NAFLD patients or general population is described.</t>
+          <t>No comparison group involving non-NAFLD patients or general population is described in relation to cancer outcomes.</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Outcomes focus on liver fibrosis progression rather than the incidence of extra-hepatic cancers.</t>
+          <t>The outcome focuses on liver fibrosis progression rather than the incidence of extra-hepatic cancers.</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>The study design is not explicitly stated as retrospective cohort; it appears to be a narrative review.</t>
+          <t>The study design description is unclear; it appears to be a narrative review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U2" t="b">
@@ -652,7 +652,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>The abstract discusses the effects of moderate alcohol consumption on NAFLD progression (liver fibrosis) but does not address extra-hepatic cancer outcomes or compare NAFLD patients to non-NAFLD/general populations. It is a review, not a retrospective cohort study.</t>
         </is>
       </c>
       <c r="W2" t="b">
@@ -695,7 +695,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>focuses on liver disease in children, not NAFLD or extra-hepatic cancers</t>
+          <t>focuses on liver disease in children, not specifically NAFLD</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -728,17 +728,17 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>This abstract focuses on pediatric liver diseases and diagnostic approaches, not NAFLD or its association with extra-hepatic cancers. It lacks relevance to the PICOS criteria entirely.</t>
+          <t>This abstract provides an overview of pediatric liver diseases, including NAFLD, but does not investigate extra-hepatic cancers or include a comparison group. It lacks relevance to the PICOS criteria for cancer incidence in NAFLD patients.</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>The population includes children with liver disease, which is outside the scope of adult NAFLD patients.</t>
+          <t>The population includes children with liver diseases, but there is no specific mention of NAFLD patients in the context of cancer risks.</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>The intervention involves diagnostic evaluations for liver disease, not NAFLD management or observation.</t>
+          <t>The intervention involves diagnosing liver disease in children, which is unrelated to managing NAFLD or observing cancer risks.</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -748,12 +748,12 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Outcomes relate to diagnosing liver disease complications, not extra-hepatic cancer incidence.</t>
+          <t>The outcomes focus on liver function tests and diagnostic methods, not extra-hepatic cancer incidence.</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>The study design is not specified as retrospective cohort; it appears to be a clinical review.</t>
+          <t>The study design appears to be a narrative review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U3" t="b">
@@ -761,7 +761,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Focuses on pediatric liver disease presentations and diagnostic considerations. No mention of NAFLD-related extra-hepatic cancer outcomes or comparisons to non-NAFLD populations. Study design is not specified as retrospective cohort.</t>
         </is>
       </c>
       <c r="W3" t="b">
@@ -804,7 +804,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>does not mention NAFLD or extra-hepatic cancers</t>
+          <t>does not mention NAFLD or any relevant outcomes</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -837,17 +837,17 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>The abstract examines transporter alterations in gastrointestinal and kidney functions due to liver dysfunction but does not address NAFLD patients or their risk of extra-hepatic cancers. It lacks a relevant population and outcome.</t>
+          <t>The abstract explores transporter alterations in gastrointestinal and kidney functions due to liver dysfunction but does not address NAFLD patients' cancer risks or provide a relevant comparison group. It lacks alignment with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>The population involves individuals with liver dysfunction broadly, not specifically NAFLD patients.</t>
+          <t>The population involves patients with liver dysfunction, but NAFLD-specific patients are not highlighted in the context of cancer risks.</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>The intervention focuses on changes in transporter functions, not NAFLD management or observation.</t>
+          <t>The intervention pertains to studying transporter alterations, which is unrelated to NAFLD management or observation of cancer risks.</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -857,12 +857,12 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Outcomes pertain to drug pharmacokinetics and endogenous compound handling, not cancer incidence.</t>
+          <t>The outcomes focus on drug pharmacokinetics and transporter functions, not extra-hepatic cancer incidence.</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>The study design is not explicitly stated as retrospective cohort; it appears to be a literature review.</t>
+          <t>The study design appears to be a literature review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U4" t="b">
@@ -870,7 +870,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Explores transporter alterations in liver failure and their pharmacokinetic implications. No direct link to NAFLD, extra-hepatic cancers, or required comparisons. Study design is not relevant.</t>
         </is>
       </c>
       <c r="W4" t="b">
@@ -913,7 +913,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>does not provide specific data from a cohort study</t>
+          <t>is a review, not a cohort study, and lacks comparison data</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -928,12 +928,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>extrahepatic malignancies</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>risk of extrahepatic complications including cancers</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>This abstract directly addresses NAFLD patients and their increased risk of extra-hepatic malignancies, including colorectal cancer. It compares NAFLD patients to broader health risks and aligns with the PICOS criteria.</t>
+          <t>This abstract directly addresses extra-hepatic complications of NAFLD, including various cancers such as colorectal cancer. It mentions the need for collaborative care and screening methods, aligning well with the PICOS criteria despite lacking detailed study design information.</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The study design is described as a narrative review, which may not fully meet the retrospective cohort requirement but still provides valuable insights into NAFLD-related cancer risks.</t>
         </is>
       </c>
       <c r="U5" t="b">
@@ -979,7 +979,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Identifies extrahepatic cancers (e.g., colorectal cancer) as a complication of NAFLD but is a narrative review, not a retrospective cohort study. Model A correctly noted the design mismatch; Model B overemphasized outcome relevance without addressing study design.</t>
         </is>
       </c>
       <c r="W5" t="b">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>does not mention NAFLD or extra-hepatic cancers</t>
+          <t>does not mention NAFLD or any relevant outcomes</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1055,17 +1055,17 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>The abstract focuses on sphingolipids and ER stress mechanisms without addressing NAFLD patients or their risk of extra-hepatic cancers. It lacks relevance to the PICOS criteria.</t>
+          <t>The abstract focuses on sphingolipids and ER stress mechanisms without addressing NAFLD patients' cancer risks or providing a relevant comparison group. It lacks alignment with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>The population is not specified as NAFLD patients; it discusses cellular mechanisms broadly.</t>
+          <t>The population is not specified as NAFLD patients in the context of cancer risks.</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>The intervention involves studying sphingolipids and ER stress, not NAFLD management or observation.</t>
+          <t>The intervention involves studying sphingolipids and ER stress, which is unrelated to NAFLD management or observation of cancer risks.</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1075,12 +1075,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Outcomes relate to ER stress and sphingolipid roles, not cancer incidence.</t>
+          <t>The outcomes focus on ER stress and sphingolipid roles, not extra-hepatic cancer incidence.</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>The study design is not explicitly stated as retrospective cohort; it appears to be a mechanistic review.</t>
+          <t>The study design appears to be a narrative review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U6" t="b">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Focuses on ER stress and sphingolipids in cellular processes, unrelated to NAFLD, cancer outcomes, or required comparisons. Both models correctly excluded it.</t>
         </is>
       </c>
       <c r="W6" t="b">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>does not mention NAFLD or extra-hepatic cancers</t>
+          <t>does not mention NAFLD or any relevant outcomes</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1164,17 +1164,17 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>The abstract reviews epigenetic mechanisms in gene expression regulation but does not address NAFLD patients or their risk of extra-hepatic cancers. It lacks relevance to the PICOS criteria.</t>
+          <t>The abstract discusses epigenetic mechanisms and their role in gene expression regulation but does not address NAFLD patients' cancer risks or provide a relevant comparison group. It lacks alignment with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>The population is not specified as NAFLD patients; it discusses epigenetic regulation broadly.</t>
+          <t>The population is not specified as NAFLD patients in the context of cancer risks.</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>The intervention involves studying epigenetic events, not NAFLD management or observation.</t>
+          <t>The intervention involves studying epigenetic events, which is unrelated to NAFLD management or observation of cancer risks.</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1184,12 +1184,12 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Outcomes relate to epigenetic regulation, not cancer incidence.</t>
+          <t>The outcomes focus on epigenetic regulation, not extra-hepatic cancer incidence.</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>The study design is not explicitly stated as retrospective cohort; it appears to be a mechanistic review.</t>
+          <t>The study design appears to be a narrative review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U7" t="b">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Discusses epigenetics broadly, with no mention of NAFLD, cancer outcomes, or relevant comparisons. Both models agreed on exclusion.</t>
         </is>
       </c>
       <c r="W7" t="b">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>matches all PICOS criteria with relevant outcomes</t>
+          <t>matches all PICOS criteria with relevant outcomes and comparisons</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>This abstract provides a meta-analysis of NAFLD patients and their increased risk of colorectal polyps, which are precursors to colorectal cancer. It compares NAFLD patients to non-NAFLD populations and aligns with the PICOS criteria.</t>
+          <t>This abstract examines the association between NAFLD and colorectal polyps, including adenomas and cancers, using observational studies. It provides gender-specific risk analysis, aligning well with the PICOS criteria despite some heterogeneity in study types.</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Meta-analysis of observational studies (including cohorts) linking NAFLD to colorectal polyps/adenomas. While outcomes partially align, the study design is a meta-analysis, not a retrospective cohort. Model A correctly excluded based on design; Model B overlooked this limitation.</t>
         </is>
       </c>
       <c r="W8" t="b">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>does not mention NAFLD or extra-hepatic cancers</t>
+          <t>does not mention NAFLD or relevant outcomes</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>review of literature</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="N11" t="b">
@@ -1592,17 +1592,17 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>The abstract discusses scutellarin's pharmacological effects, including anti-tumor properties, but does not focus on NAFLD patients or their risk of extra-hepatic cancers. It lacks relevance to the PICOS criteria.</t>
+          <t>The abstract discusses scutellarin's pharmacological effects, including anti-tumor properties, but does not specifically address NAFLD patients' cancer risks or provide a relevant comparison group. It lacks alignment with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>The population is not specified as NAFLD patients; it discusses scutellarin's effects broadly.</t>
+          <t>The population is not specified as NAFLD patients in the context of cancer risks.</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>The intervention involves studying scutellarin's mechanisms, not NAFLD management or observation.</t>
+          <t>The intervention involves studying scutellarin's effects, which is unrelated to NAFLD management or observation of cancer risks.</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1612,12 +1612,12 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Outcomes relate to scutellarin's pharmacological actions, not cancer incidence.</t>
+          <t>The outcomes focus on scutellarin's mechanisms, not extra-hepatic cancer incidence.</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>The study design is not explicitly stated as retrospective cohort; it appears to be a mechanistic review.</t>
+          <t>The study design appears to be a narrative review rather than a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U11" t="b">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Reviews scutellarin's anti-tumor mechanisms (including colorectal cancer) and metabolic effects in NAFLD. However, it is a review of pharmacological actions, not a retrospective cohort study. Both models agreed on exclusion.</t>
         </is>
       </c>
       <c r="W11" t="b">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Does not address NAFLD, intervention, comparison, outcomes, or study design.</t>
+          <t>does not address NAFLD or related outcomes</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>curcumin applications for health promotion</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1806,27 +1806,27 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>The abstract focuses on curcumin's biological activities and health benefits but does not specifically address NAFLD or its association with extra-hepatic cancers. The population, intervention, comparison, and outcomes are unrelated to the PICOS criteria.</t>
+          <t>The abstract discusses curcumin's biological activities and its potential health benefits but does not focus on NAFLD or extra-hepatic cancer outcomes. It lacks a defined population, intervention, comparison, or relevant outcomes, making it irrelevant to the PICOS criteria.</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>The abstract discusses general health promotion rather than patients with NAFLD.</t>
+          <t>The abstract does not specify a population related to NAFLD or cancer.</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>The intervention pertains to curcumin's effects rather than observation or management of NAFLD.</t>
+          <t>There is no mention of an intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>No comparison group relevant to NAFLD or general population is mentioned.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Outcomes focus on antioxidant, anti-inflammatory, and other health effects, not extra-hepatic cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers or NAFLD are not addressed.</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Abstract focuses on curcumin's general biological activities and health applications, including hepatoprotective effects, but does not address NAFLD patients, cancer incidence outcomes, or retrospective cohort design. It is a review article, not a study meeting PICOS criteria.</t>
         </is>
       </c>
       <c r="W13" t="b">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Does not focus on NAFLD or specified interventions and comparisons.</t>
+          <t>does not focus on NAFLD management or cancer outcomes</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>effects of intestinal fungi on health</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>correlation with colorectal cancer and liver diseases</t>
+          <t>correlation with various diseases including NAFLD</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1915,27 +1915,27 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Although the abstract mentions intestinal fungi's role in metabolism-associated fatty liver disease, it does not provide specific data on NAFLD patients or their risk of extra-hepatic cancers. The PICOS elements are incomplete or irrelevant.</t>
+          <t>While the abstract mentions intestinal fungi and their association with diseases including NAFLD, it does not specifically address extra-hepatic cancer outcomes or provide details on interventions or comparisons. The study design is also a review, not a retrospective cohort study.</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>The population includes individuals with various diseases but does not specify NAFLD patients.</t>
+          <t>The population includes individuals with various diseases but does not focus specifically on NAFLD patients.</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>The intervention involves fungi-bacteria interactions rather than NAFLD management.</t>
+          <t>There is no specific intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>No direct comparison between NAFLD and non-NAFLD groups is provided.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Outcomes relate to intestinal fungi's effects on diseases, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Discusses intestinal fungi's role in diseases (including metabolism-associated fatty liver disease) but does not specifically study NAFLD patients, compare cancer incidence outcomes, or use a retrospective cohort design. It is a review of correlations, not an original study.</t>
         </is>
       </c>
       <c r="W14" t="b">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Does not address NAFLD, intervention, comparison, outcomes, or study design.</t>
+          <t>does not involve NAFLD or cancer outcomes</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>patients with LMNA variants</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>various clinical manifestations</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -2024,32 +2024,32 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>The abstract describes a progeroid syndrome caused by LMNA variants but does not address NAFLD or its association with extra-hepatic cancers. None of the PICOS criteria are met.</t>
+          <t>The abstract focuses on LMNA variants and multisystem progeroid syndrome, which is unrelated to NAFLD or extra-hepatic cancer outcomes. The population, intervention, and outcomes do not align with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>The population consists of patients with LMNA p.R349W variant, not NAFLD patients.</t>
+          <t>The population involves patients with LMNA variants, not NAFLD.</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>The intervention involves functional studies on fibroblasts, not NAFLD management.</t>
+          <t>There is no intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>No comparison group related to NAFLD or general population is described.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Outcomes focus on lipodystrophy and cardiomyopathy, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>The study design includes case reports and functional studies, not a retrospective cohort study.</t>
+          <t>The study design is a case series, not a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U15" t="b">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Describes a genetic progeroid syndrome with hepatomegaly but does not address NAFLD, cancer outcomes, or retrospective cohort design. Focus is on LMNA variant-related multisystem disorders, not NAFLD management or cancer risk.</t>
         </is>
       </c>
       <c r="W15" t="b">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Does not address NAFLD, intervention, comparison, outcomes, or study design.</t>
+          <t>does not address NAFLD or related outcomes</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>influence of sex and gender on health</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -2133,27 +2133,27 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>The abstract discusses sex and gender disparities in disease but does not focus on NAFLD or its link to extra-hepatic cancers. The PICOS criteria are not addressed.</t>
+          <t>The abstract discusses sex and gender disparities in disease but does not focus on NAFLD or extra-hepatic cancer outcomes. It lacks a defined population, intervention, comparison, or relevant outcomes, making it irrelevant to the PICOS criteria.</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>The population is general and not specific to NAFLD patients.</t>
+          <t>The population is not specified as NAFLD patients.</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>The intervention pertains to sex and gender influences, not NAFLD management.</t>
+          <t>There is no intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>No comparison group involving NAFLD or general population is mentioned.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Outcomes relate to sex and gender disparities, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Broadly reviews sex/gender disparities in health outcomes without specific focus on NAFLD, cancer incidence, or retrospective cohort studies. Irrelevant to PICOS criteria.</t>
         </is>
       </c>
       <c r="W16" t="b">
@@ -2209,17 +2209,17 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Focuses on breast cancer, not NAFLD as population.</t>
+          <t>focuses on breast cancer, not NAFLD management or cancer incidence</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>premenopausal breast cancer patients</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>comparison of TOR and TAM in breast cancer</t>
+          <t>comparison of TOR and TAM treatments</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>incidence of ovarian cysts and fatty liver</t>
+          <t>incidence of fatty liver and other side effects</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2242,17 +2242,17 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>The abstract compares the safety of two drugs in breast cancer patients but does not address NAFLD or its association with extra-hepatic cancers. The PICOS criteria are not fulfilled.</t>
+          <t>The abstract compares the safety of two drugs in premenopausal breast cancer patients, which is unrelated to NAFLD or extra-hepatic cancer outcomes. The population, intervention, and outcomes do not align with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>The population includes premenopausal breast cancer patients, not NAFLD patients.</t>
+          <t>The population involves premenopausal breast cancer patients, not NAFLD patients.</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>The intervention involves drug safety comparisons, not NAFLD management.</t>
+          <t>The intervention involves drug treatment for breast cancer, not NAFLD management.</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2262,12 +2262,12 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Outcomes focus on ovarian cysts and endometrial thickening, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>The study design is a prospective randomized clinical trial, not a retrospective cohort study.</t>
+          <t>The study design is a randomized clinical trial, not a retrospective cohort study.</t>
         </is>
       </c>
       <c r="U17" t="b">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Compares Toremifene and Tamoxifen in premenopausal breast cancer patients, mentioning fatty liver as a side effect. Population is not NAFLD patients, and study design is a prospective randomized trial, not a retrospective cohort. Outcomes are drug safety, not cancer incidence.</t>
         </is>
       </c>
       <c r="W17" t="b">
@@ -2318,17 +2318,17 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>While mentioning NAFLD, it does not provide a direct comparison or specific outcomes related to extra-hepatic cancers.</t>
+          <t>discusses liver diseases in pregnancy, not specifically NAFLD or cancer outcomes</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>patients with liver diseases including NAFLD</t>
+          <t>pregnant women with liver diseases</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>management of liver diseases in pregnancy</t>
+          <t>management of liver diseases</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>The abstract reviews liver diseases during pregnancy, including NAFLD, but does not examine the incidence of extra-hepatic cancers. The PICOS criteria are incomplete.</t>
+          <t>The abstract reviews liver diseases during pregnancy, including NAFLD, but does not focus on extra-hepatic cancer outcomes or provide details on interventions or comparisons. The study design is a review, not a retrospective cohort study.</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2361,17 +2361,17 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>The intervention pertains to managing liver diseases in pregnancy, not NAFLD management.</t>
+          <t>There is no specific intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>No comparison group involving NAFLD or general population is provided.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Outcomes focus on maternal and fetal health, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Discusses liver diseases in pregnancy (including NAFLD) but focuses on maternal/fetal outcomes, not cancer incidence. Study design is a review, not a retrospective cohort. Does not meet PICOS criteria.</t>
         </is>
       </c>
       <c r="W18" t="b">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Does not address NAFLD, intervention, comparison, outcomes, or study design.</t>
+          <t>does not address NAFLD or related outcomes</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>overview of F. prausnitzii features</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>correlation with intestinal disorders</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -2460,27 +2460,27 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>The abstract discusses Faecalibacterium prausnitzii's role in intestinal health but does not address NAFLD or its association with extra-hepatic cancers. The PICOS criteria are not met.</t>
+          <t>The abstract discusses Faecalibacterium prausnitzii and its role in intestinal health but does not focus on NAFLD or extra-hepatic cancer outcomes. It lacks a defined population, intervention, comparison, or relevant outcomes, making it irrelevant to the PICOS criteria.</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>The population is general and not specific to NAFLD patients.</t>
+          <t>The population is not specified as NAFLD patients.</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>The intervention involves F. prausnitzii's effects, not NAFLD management.</t>
+          <t>There is no intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>No comparison group involving NAFLD or general population is mentioned.</t>
+          <t>No comparison group involving NAFLD or general population is described.</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Outcomes relate to intestinal disorders, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Reviews Faecalibacterium prausnitzii's role in gut health and disease correlations but lacks NAFLD population, cancer outcomes, or retrospective cohort design. Irrelevant to PICOS.</t>
         </is>
       </c>
       <c r="W19" t="b">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Does not address NAFLD, intervention, comparison, outcomes, or study design.</t>
+          <t>focuses on CKD, not NAFLD or cancer incidence</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>targeting senescent cells for CKD</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>role of cellular senescence in kidney fibrosis</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2569,17 +2569,17 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>The abstract focuses on cellular senescence in chronic kidney disease but does not address NAFLD or its link to extra-hepatic cancers. The PICOS criteria are not fulfilled.</t>
+          <t>The abstract focuses on cellular senescence in chronic kidney disease, which is unrelated to NAFLD or extra-hepatic cancer outcomes. The population, intervention, and outcomes do not align with the PICOS criteria.</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>The population includes individuals with chronic kidney disease, not NAFLD patients.</t>
+          <t>The population involves patients with chronic kidney disease, not NAFLD patients.</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>The intervention pertains to senescence mechanisms, not NAFLD management.</t>
+          <t>There is no intervention related to NAFLD management or observation.</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Outcomes focus on kidney fibrosis, not cancer incidence.</t>
+          <t>Outcomes related to extra-hepatic cancers are not addressed.</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>API call failed or returned no results</t>
+          <t>Focuses on cellular senescence in kidney fibrosis and CKD, unrelated to NAFLD or cancer outcomes. Study design is a review, not a retrospective cohort.</t>
         </is>
       </c>
       <c r="W20" t="b">

</xml_diff>